<commit_message>
Added codes for paper: lasso GLM and lasso GLMM
</commit_message>
<xml_diff>
--- a/dat/cases/hk_annual_cases.xlsx
+++ b/dat/cases/hk_annual_cases.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (NHRI Taiwan)\Workspace\Github\DengueForecastHK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\dengue-forecast-hk\dat\cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20022" windowHeight="8227"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20025" windowHeight="8220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -350,12 +350,12 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -363,15 +363,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2002</v>
       </c>
       <c r="B2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2003</v>
       </c>
@@ -379,7 +379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2004</v>
       </c>
@@ -387,7 +387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2005</v>
       </c>
@@ -395,7 +395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2006</v>
       </c>
@@ -403,7 +403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2007</v>
       </c>
@@ -411,7 +411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2008</v>
       </c>
@@ -419,7 +419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2009</v>
       </c>
@@ -427,7 +427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2010</v>
       </c>
@@ -435,7 +435,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2011</v>
       </c>
@@ -443,7 +443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2012</v>
       </c>
@@ -451,7 +451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2013</v>
       </c>
@@ -459,7 +459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2014</v>
       </c>
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2015</v>
       </c>
@@ -475,7 +475,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2016</v>
       </c>
@@ -483,7 +483,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2017</v>
       </c>
@@ -491,7 +491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2018</v>
       </c>

</xml_diff>